<commit_message>
moved the logic that extracts the data from the table in RMSE and put it in RMSEUtils. Will do this for the other mechanisms as well
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/f11_95RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/f11_95RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Desktop\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\OTIS_Four_Bar\RMSE_Results\E\AngVel\f11_95RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60012053-8824-41E6-92BA-A90E9568EE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C17434-1143-4B82-8175-9D09EF59B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D96D8101-076C-4FDC-96F4-33B3BB214610}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{377293E5-301E-4BCD-9117-25B2A74DC99D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1684BB6E-CA17-4B14-A2E4-40524781040B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916D616-0A96-4C07-959F-E9E2549B8CF5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Cleaned up the logic within RMSEUtils
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/f11_95RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/f11_95RPM/RMSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Desktop\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\OTIS_Four_Bar\RMSE_Results\E\AngVel\f11_95RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C17434-1143-4B82-8175-9D09EF59B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461DB853-B4FA-478E-8558-5CE9CA5CB82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{377293E5-301E-4BCD-9117-25B2A74DC99D}"/>
+    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{0202C2F6-0460-4A8E-B6B2-B9BEE75CFD18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916D616-0A96-4C07-959F-E9E2549B8CF5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC3CA17-BB0C-4C14-8D39-754C5C974D6C}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
showcase theoretical and experimental data from RMSEUtils to RMSE to easily track this data overtime
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/f11_95RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/f11_95RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Desktop\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\OTIS_Four_Bar\RMSE_Results\E\AngVel\f11_95RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461DB853-B4FA-478E-8558-5CE9CA5CB82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE552EC-06C3-469F-A589-5F19F371B85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{0202C2F6-0460-4A8E-B6B2-B9BEE75CFD18}"/>
+    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{1E0ED030-27E0-4D8A-A9C2-2F43964B99A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC3CA17-BB0C-4C14-8D39-754C5C974D6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA013D9-F491-44E5-866D-47DD0975A2E0}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>